<commit_message>
1. Can select last update date 2. Can locate stock by name or number 3. Can show all stock by set period = 0
</commit_message>
<xml_diff>
--- a/Requirement/All Requirement.xlsx
+++ b/Requirement/All Requirement.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>爬下一点仓位或者东方财富的所有股票的股东信息，保存至本地数据库</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -24,40 +24,56 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>需求</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>序号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>c#程序读取数据库，列出连续减少N期的股票
-单击股票后，右边列出K线图，分时线，公积金，流通盘等</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一点仓位OK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>未开始</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>未开始</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需求</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>序号</t>
+单击股票后，右边列出每期的股东人数信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以选择最后一期的日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续减少期数设为0，表示列出所有股票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>输入号码和股票名可以定位股票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +94,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -85,6 +102,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -92,6 +110,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -136,7 +155,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -152,7 +171,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -441,28 +460,28 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.375" style="6" customWidth="1"/>
     <col min="2" max="2" width="67.375" customWidth="1"/>
     <col min="3" max="3" width="34.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="18.75">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -470,10 +489,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -481,141 +500,162 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>

</xml_diff>